<commit_message>
Updating stock assessment inputs and trying continous color scales instead of discrete
</commit_message>
<xml_diff>
--- a/tables/table_1.xlsx
+++ b/tables/table_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brendan/Documents/R/Github/calcofi_spf/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Brendan/Documents/R/Github/calcofi_spf/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F243D838-9A41-EA43-AD6C-3A942273EB9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D48E681-E82D-7546-AA36-A760D67CA929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{4F29BB74-2739-D84A-A2C9-F20B78BA2196}"/>
   </bookViews>
@@ -61,7 +61,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,24 +71,13 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -116,17 +105,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,121 +434,121 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="1" max="1" width="20" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="14" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>0.85721500721500699</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="4">
         <v>2E-16</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="3">
         <v>0.40389140271493201</v>
       </c>
-      <c r="D4" s="7">
-        <v>3.5210040411020899E-3</v>
+      <c r="D4" s="8">
+        <v>4.0976178513504298E-3</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="3">
         <v>0.31910858226647698</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="8">
         <v>5.4700484464831799E-2</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4" t="s">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="3">
         <v>-0.44072009775920601</v>
       </c>
-      <c r="D8" s="7">
-        <v>5.6166443766418198E-3</v>
+      <c r="D8" s="8">
+        <v>5.2947460299647801E-3</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K13" s="1"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K16" s="2"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
     </row>
     <row r="17" spans="11:13" x14ac:dyDescent="0.2">
-      <c r="K17" s="2"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>